<commit_message>
Update Scenarios with actors.xlsx
</commit_message>
<xml_diff>
--- a/Scenarios with actors.xlsx
+++ b/Scenarios with actors.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721A4A9E-F90B-4827-A920-319175B5CD8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -108,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -325,17 +326,17 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="9"/>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="%40 - Vurgu3" xfId="6" builtinId="39"/>
-    <cellStyle name="%60 - Vurgu2" xfId="5" builtinId="36"/>
-    <cellStyle name="%60 - Vurgu4" xfId="7" builtinId="44"/>
-    <cellStyle name="%60 - Vurgu5" xfId="8" builtinId="48"/>
-    <cellStyle name="%60 - Vurgu6" xfId="10" builtinId="52"/>
-    <cellStyle name="Çıkış" xfId="3" builtinId="21"/>
-    <cellStyle name="İşaretli Hücre" xfId="4" builtinId="23"/>
-    <cellStyle name="İyi" xfId="1" builtinId="26"/>
-    <cellStyle name="Kötü" xfId="2" builtinId="27"/>
+    <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="5" builtinId="36"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="60% - Accent5" xfId="8" builtinId="48"/>
+    <cellStyle name="60% - Accent6" xfId="10" builtinId="52"/>
+    <cellStyle name="Accent6" xfId="9" builtinId="49"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Vurgu6" xfId="9" builtinId="49"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -612,11 +613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,6 +760,7 @@
       <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -782,6 +784,7 @@
       <c r="E11" s="13" t="s">
         <v>15</v>
       </c>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -841,6 +844,7 @@
       <c r="E16" s="13" t="s">
         <v>15</v>
       </c>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">

</xml_diff>

<commit_message>
Scenarios finished for now
</commit_message>
<xml_diff>
--- a/Scenarios with actors.xlsx
+++ b/Scenarios with actors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Admin</t>
   </si>
@@ -103,13 +103,16 @@
   </si>
   <si>
     <t>The number of scenarios written is more or equal to the number of the use-cases related to the spesific scenario.</t>
+  </si>
+  <si>
+    <t>Number of Scenarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +170,15 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -237,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -275,8 +287,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -288,8 +315,9 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -323,14 +351,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="11" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="%40 - Vurgu3" xfId="6" builtinId="39"/>
     <cellStyle name="%60 - Vurgu2" xfId="5" builtinId="36"/>
     <cellStyle name="%60 - Vurgu4" xfId="7" builtinId="44"/>
     <cellStyle name="%60 - Vurgu5" xfId="8" builtinId="48"/>
     <cellStyle name="%60 - Vurgu6" xfId="10" builtinId="52"/>
     <cellStyle name="Çıkış" xfId="3" builtinId="21"/>
+    <cellStyle name="Hesaplama" xfId="11" builtinId="22"/>
     <cellStyle name="İşaretli Hücre" xfId="4" builtinId="23"/>
     <cellStyle name="İyi" xfId="1" builtinId="26"/>
     <cellStyle name="Kötü" xfId="2" builtinId="27"/>
@@ -616,7 +648,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,6 +659,7 @@
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
     <col min="12" max="12" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -649,6 +682,9 @@
       <c r="F1" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="L1" s="4" t="s">
         <v>27</v>
       </c>
@@ -664,6 +700,9 @@
         <v>5</v>
       </c>
       <c r="F2" s="8"/>
+      <c r="G2" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -676,6 +715,9 @@
         <v>7</v>
       </c>
       <c r="F3" s="8"/>
+      <c r="G3" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -688,6 +730,9 @@
         <v>5</v>
       </c>
       <c r="F4" s="8"/>
+      <c r="G4" s="15">
+        <v>1</v>
+      </c>
       <c r="L4" s="7" t="s">
         <v>5</v>
       </c>
@@ -703,6 +748,9 @@
         <v>10</v>
       </c>
       <c r="F5" s="12"/>
+      <c r="G5" s="15">
+        <v>2</v>
+      </c>
       <c r="L5" s="10" t="s">
         <v>7</v>
       </c>
@@ -718,6 +766,9 @@
         <v>7</v>
       </c>
       <c r="F6" s="8"/>
+      <c r="G6" s="15">
+        <v>1</v>
+      </c>
       <c r="L6" s="11" t="s">
         <v>10</v>
       </c>
@@ -733,6 +784,9 @@
         <v>5</v>
       </c>
       <c r="F7" s="8"/>
+      <c r="G7" s="15">
+        <v>2</v>
+      </c>
       <c r="L7" s="13" t="s">
         <v>15</v>
       </c>
@@ -748,6 +802,9 @@
         <v>7</v>
       </c>
       <c r="F8" s="8"/>
+      <c r="G8" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -759,6 +816,9 @@
       <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -771,6 +831,9 @@
         <v>10</v>
       </c>
       <c r="F10" s="14"/>
+      <c r="G10" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -782,6 +845,9 @@
       <c r="E11" s="13" t="s">
         <v>15</v>
       </c>
+      <c r="G11" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -794,6 +860,9 @@
         <v>7</v>
       </c>
       <c r="F12" s="8"/>
+      <c r="G12" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -805,7 +874,9 @@
       <c r="E13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="12"/>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -818,6 +889,9 @@
         <v>5</v>
       </c>
       <c r="F14" s="8"/>
+      <c r="G14" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -830,6 +904,9 @@
         <v>10</v>
       </c>
       <c r="F15" s="12"/>
+      <c r="G15" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -841,8 +918,11 @@
       <c r="E16" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>23</v>
       </c>
@@ -852,8 +932,12 @@
       <c r="E17" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="14"/>
+      <c r="G17" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>24</v>
       </c>
@@ -864,8 +948,12 @@
         <v>10</v>
       </c>
       <c r="F18" s="14"/>
+      <c r="G18" s="15">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Add files via upload"
This reverts commit 5ca3b7c8932ae9aa2feea47a2b2a258d43b4c9f5.
</commit_message>
<xml_diff>
--- a/Scenarios with actors.xlsx
+++ b/Scenarios with actors.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721A4A9E-F90B-4827-A920-319175B5CD8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Admin</t>
   </si>
@@ -104,13 +103,16 @@
   </si>
   <si>
     <t>The number of scenarios written is more or equal to the number of the use-cases related to the spesific scenario.</t>
+  </si>
+  <si>
+    <t>Number of Scenarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +170,15 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -238,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -276,8 +287,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -289,8 +315,9 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -324,19 +351,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="11" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
-    <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="5" builtinId="36"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="60% - Accent5" xfId="8" builtinId="48"/>
-    <cellStyle name="60% - Accent6" xfId="10" builtinId="52"/>
-    <cellStyle name="Accent6" xfId="9" builtinId="49"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="12">
+    <cellStyle name="%40 - Vurgu3" xfId="6" builtinId="39"/>
+    <cellStyle name="%60 - Vurgu2" xfId="5" builtinId="36"/>
+    <cellStyle name="%60 - Vurgu4" xfId="7" builtinId="44"/>
+    <cellStyle name="%60 - Vurgu5" xfId="8" builtinId="48"/>
+    <cellStyle name="%60 - Vurgu6" xfId="10" builtinId="52"/>
+    <cellStyle name="Çıkış" xfId="3" builtinId="21"/>
+    <cellStyle name="Hesaplama" xfId="11" builtinId="22"/>
+    <cellStyle name="İşaretli Hücre" xfId="4" builtinId="23"/>
+    <cellStyle name="İyi" xfId="1" builtinId="26"/>
+    <cellStyle name="Kötü" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="3" builtinId="21"/>
+    <cellStyle name="Vurgu6" xfId="9" builtinId="49"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -613,11 +644,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +659,7 @@
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
     <col min="12" max="12" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -650,6 +682,9 @@
       <c r="F1" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="L1" s="4" t="s">
         <v>27</v>
       </c>
@@ -665,6 +700,9 @@
         <v>5</v>
       </c>
       <c r="F2" s="8"/>
+      <c r="G2" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -677,6 +715,9 @@
         <v>7</v>
       </c>
       <c r="F3" s="8"/>
+      <c r="G3" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -689,6 +730,9 @@
         <v>5</v>
       </c>
       <c r="F4" s="8"/>
+      <c r="G4" s="15">
+        <v>1</v>
+      </c>
       <c r="L4" s="7" t="s">
         <v>5</v>
       </c>
@@ -704,6 +748,9 @@
         <v>10</v>
       </c>
       <c r="F5" s="12"/>
+      <c r="G5" s="15">
+        <v>2</v>
+      </c>
       <c r="L5" s="10" t="s">
         <v>7</v>
       </c>
@@ -719,6 +766,9 @@
         <v>7</v>
       </c>
       <c r="F6" s="8"/>
+      <c r="G6" s="15">
+        <v>1</v>
+      </c>
       <c r="L6" s="11" t="s">
         <v>10</v>
       </c>
@@ -734,6 +784,9 @@
         <v>5</v>
       </c>
       <c r="F7" s="8"/>
+      <c r="G7" s="15">
+        <v>2</v>
+      </c>
       <c r="L7" s="13" t="s">
         <v>15</v>
       </c>
@@ -749,6 +802,9 @@
         <v>7</v>
       </c>
       <c r="F8" s="8"/>
+      <c r="G8" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
@@ -760,7 +816,9 @@
       <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -773,6 +831,9 @@
         <v>10</v>
       </c>
       <c r="F10" s="14"/>
+      <c r="G10" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -784,7 +845,9 @@
       <c r="E11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="G11" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -797,6 +860,9 @@
         <v>7</v>
       </c>
       <c r="F12" s="8"/>
+      <c r="G12" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -808,7 +874,9 @@
       <c r="E13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="12"/>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -821,6 +889,9 @@
         <v>5</v>
       </c>
       <c r="F14" s="8"/>
+      <c r="G14" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -833,6 +904,9 @@
         <v>10</v>
       </c>
       <c r="F15" s="12"/>
+      <c r="G15" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -844,9 +918,11 @@
       <c r="E16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>23</v>
       </c>
@@ -856,8 +932,12 @@
       <c r="E17" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="14"/>
+      <c r="G17" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>24</v>
       </c>
@@ -868,8 +948,12 @@
         <v>10</v>
       </c>
       <c r="F18" s="14"/>
+      <c r="G18" s="15">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>